<commit_message>
Bijna klaar met deverneuking Meten aan de robot
</commit_message>
<xml_diff>
--- a/docs/meten-aan-de-robot/meetresultaten/meetresultaten-en-verwerking.xlsx
+++ b/docs/meten-aan-de-robot/meetresultaten/meetresultaten-en-verwerking.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Kalibratie</t>
   </si>
@@ -62,6 +62,15 @@
   <si>
     <t>Gemiddeldes</t>
   </si>
+  <si>
+    <t>Stdev(v)</t>
+  </si>
+  <si>
+    <t>stdev(s)</t>
+  </si>
+  <si>
+    <t>Verwachtte tijd 25 cm.</t>
+  </si>
 </sst>
 </file>
 
@@ -99,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -157,18 +167,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:trendline>
-            <c:name>RE</c:name>
-            <c:spPr>
-              <a:ln>
-                <a:prstDash val="lgDash"/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:intercept val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Blad1!$J$5:$J$9</c:f>
@@ -230,18 +228,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:trendline>
-            <c:name>TL</c:name>
-            <c:spPr>
-              <a:ln>
-                <a:prstDash val="dash"/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:intercept val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Blad1!$J$5:$J$9</c:f>
@@ -303,18 +289,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:trendline>
-            <c:name>JC</c:name>
-            <c:spPr>
-              <a:ln>
-                <a:prstDash val="lgDashDot"/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:intercept val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Blad1!$J$5:$J$9</c:f>
@@ -359,6 +333,153 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.8541735999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>RE snelheid</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad1!$O$5:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad1!$P$5:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0,000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6035024999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>TL snelheid</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad1!$O$5:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad1!$Q$5:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0,000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9022009999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>JC snelheid</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="lgDashDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad1!$O$5:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad1!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0,000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8366084999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,11 +494,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116365504"/>
-        <c:axId val="116363776"/>
+        <c:axId val="136894080"/>
+        <c:axId val="136894656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116365504"/>
+        <c:axId val="136894080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -408,13 +529,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116363776"/>
+        <c:crossAx val="136894656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116363776"/>
+        <c:axId val="136894656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.5"/>
@@ -446,7 +567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116365504"/>
+        <c:crossAx val="136894080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -457,9 +578,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.82798824675217486"/>
+          <c:x val="0.7902523976955711"/>
           <c:y val="0.50990748328404656"/>
-          <c:w val="0.10024117268360323"/>
+          <c:w val="0.1767092556826623"/>
           <c:h val="0.32729254996971535"/>
         </c:manualLayout>
       </c:layout>
@@ -806,11 +927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112924288"/>
-        <c:axId val="112923712"/>
+        <c:axId val="230064704"/>
+        <c:axId val="230065280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112924288"/>
+        <c:axId val="230064704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -841,13 +962,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112923712"/>
+        <c:crossAx val="230065280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112923712"/>
+        <c:axId val="230065280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +1005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112924288"/>
+        <c:crossAx val="230064704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1279,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:M22"/>
+  <dimension ref="A3:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1414,7 @@
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1312,17 +1433,17 @@
       <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" t="s">
+      <c r="P3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
         <v>2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="R3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1341,8 +1462,11 @@
       <c r="M4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1376,8 +1500,20 @@
       <c r="M5" s="1">
         <v>0.57506460000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1402,8 +1538,23 @@
       <c r="M6" s="1">
         <v>1.1401176</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>0.25</v>
+      </c>
+      <c r="P6">
+        <f>$O$6/B23</f>
+        <v>2.6035024999999998</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:R6" si="0">$O$6/C23</f>
+        <v>2.9022009999999998</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>2.8366084999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1429,7 +1580,7 @@
         <v>1.7318328000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1455,7 +1606,7 @@
         <v>2.3301895999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1481,7 +1632,7 @@
         <v>2.8541735999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1493,7 +1644,7 @@
         <v>1.1360319999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1520,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1535,7 +1686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1547,7 +1698,7 @@
         <v>1.131067</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1559,7 +1710,7 @@
         <v>1.1446160000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1568,96 +1719,142 @@
         <v>1.041401</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:D15" si="0">AVERAGE(C5:C14)</f>
+        <f t="shared" ref="C15:D15" si="1">AVERAGE(C5:C14)</f>
         <v>1.1608803999999999</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1346433999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <f>_xlfn.STDEV.P(B5:B14)</f>
         <v>5.2832092141045931E-3</v>
       </c>
-      <c r="C16" s="1">
-        <f t="shared" ref="C16:D16" si="1">_xlfn.STDEV.P(C5:C14)</f>
+      <c r="C16" s="2">
+        <f t="shared" ref="C16:D16" si="2">_xlfn.STDEV.P(C5:C14)</f>
         <v>1.060977937753654E-2</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
+      <c r="D16" s="2">
+        <f t="shared" si="2"/>
         <v>5.9416507504228286E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>0.23400000000000001</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D20">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>0.1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D21">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B21">
-        <f>$B$19/B15</f>
+      <c r="B23">
+        <f>$B$21/B15</f>
         <v>9.6024490085951528E-2</v>
       </c>
-      <c r="C21">
-        <f t="shared" ref="C21:D21" si="2">$B$19/C15</f>
+      <c r="C23">
+        <f>$B$21/C15</f>
         <v>8.6141518109875928E-2</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
+      <c r="D23">
+        <f>$B$21/D15</f>
         <v>8.8133417071830686E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>11</v>
       </c>
-      <c r="B22">
-        <f>B21*F5</f>
+      <c r="B24">
+        <f>B23*F5</f>
         <v>0.24222880523448703</v>
       </c>
-      <c r="C22">
-        <f t="shared" ref="C22:D22" si="3">C21*G5</f>
+      <c r="C24">
+        <f>C23*G5</f>
         <v>0.23461534021937144</v>
       </c>
-      <c r="D22">
+      <c r="D24">
+        <f>D23*H5</f>
+        <v>0.24004048320379778</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2">
+        <f>SQRT(POWER($B$21/POWER(B15,2),2)*POWER(B16,2)+POWER(1/B15,2)*POWER($D$21,2))</f>
+        <v>6.8398225831562169E-4</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:D26" si="3">SQRT(POWER($B$21/POWER(C15,2),2)*POWER(C16,2)+POWER(1/C15,2)*POWER($D$21,2))</f>
+        <v>8.973990419649259E-4</v>
+      </c>
+      <c r="D25" s="2">
         <f t="shared" si="3"/>
-        <v>0.24004048320379778</v>
+        <v>6.3811131024387759E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2">
+        <f>SQRT(POWER(B23,2)*POWER(B16,2)+POWER(B15,2)*POWER(B25,2))</f>
+        <v>8.7449530150908103E-4</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" ref="C26:D26" si="4">SQRT(POWER(C23,2)*POWER(C16,2)+POWER(C15,2)*POWER(C25,2))</f>
+        <v>1.38585056746987E-3</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="4"/>
+        <v>8.9355210690152456E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>